<commit_message>
Agrege el formato de entrega de audiencias referenciado desde el issue #1
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario del STJEM\Documents\GitHub\familiareS\audiencias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario del STJEM\Documents\GitHub\familiareS\audiencias\relacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4920" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4920" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Respaldo en Computadora" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="conteo audiencias" sheetId="6" r:id="rId5"/>
     <sheet name="firmadas fuera de tiempo" sheetId="8" r:id="rId6"/>
     <sheet name="no agendados" sheetId="9" r:id="rId7"/>
+    <sheet name="formato entrega cedetic" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="258">
   <si>
     <t>Expediente</t>
   </si>
@@ -789,6 +790,21 @@
   </si>
   <si>
     <t>560 GB</t>
+  </si>
+  <si>
+    <t>EXPE</t>
+  </si>
+  <si>
+    <t>AUDIENCIA</t>
+  </si>
+  <si>
+    <t>FECHA HORA</t>
+  </si>
+  <si>
+    <t>FOLIO</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -2393,7 +2409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -5679,4 +5695,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualize las fechas de respaldo del disco duro Este cambio es del issue #2
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4920" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4920" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Respaldo en Computadora" sheetId="1" r:id="rId1"/>
@@ -2409,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2508,7 +2508,7 @@
         <v>252</v>
       </c>
       <c r="F4" s="1">
-        <v>43335</v>
+        <v>43341</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -5701,11 +5701,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Actualize fecha de respaldo del dd
ultima fecha de respaldo del disco duro
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario del STJEM\Documents\GitHub\familiareS\audiencias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario del STJEM\Documents\GitHub\familiareS\audiencias\relacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2394,7 +2394,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2493,6 +2493,9 @@
       </c>
       <c r="F4" s="1">
         <v>43335</v>
+      </c>
+      <c r="G4" s="1">
+        <v>43369</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Respaldo en disco duro del 27/09/2018
respalde en disco duro las audiencias del juzgado al dia 27/09/2018 y respalde el contenido de la memoria para liberar espacio en disco de la pc
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="255">
   <si>
     <t>Expediente</t>
   </si>
@@ -789,6 +789,12 @@
   </si>
   <si>
     <t>560 GB</t>
+  </si>
+  <si>
+    <t>360 GB</t>
+  </si>
+  <si>
+    <t>479 GB</t>
   </si>
 </sst>
 </file>
@@ -2391,10 +2397,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2520,6 +2526,27 @@
       <c r="G5" t="s">
         <v>121</v>
       </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6">
+        <v>952</v>
+      </c>
+      <c r="C6">
+        <v>317</v>
+      </c>
+      <c r="D6" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="1">
+        <v>43371</v>
+      </c>
+      <c r="G6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fecha de ultimo respaldo en el cedetic
cambie la fecha del ultimo respaldo enviado al cedetic, ya que decia 26/09/2018 y es 26/08/2018
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -2400,7 +2400,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2501,7 +2501,7 @@
         <v>43335</v>
       </c>
       <c r="G4" s="1">
-        <v>43369</v>
+        <v>43338</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
respaldo hasta el 18/10/2018
respaldo a llevar al cedetic para respaldar desde 28/08/2018 hasta 18/10/2018
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="257">
   <si>
     <t>Expediente</t>
   </si>
@@ -795,6 +795,12 @@
   </si>
   <si>
     <t>479 GB</t>
+  </si>
+  <si>
+    <t>392 GB</t>
+  </si>
+  <si>
+    <t>416 GB</t>
   </si>
 </sst>
 </file>
@@ -2397,10 +2403,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2547,6 +2553,26 @@
         <v>43371</v>
       </c>
       <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7">
+        <v>1015</v>
+      </c>
+      <c r="C7">
+        <v>387</v>
+      </c>
+      <c r="D7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E7" t="s">
+        <v>256</v>
+      </c>
+      <c r="F7" s="1">
+        <v>43391</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Respaldo audiencias al 23/11/2018
respaldo de audiencias al 23 de noviembre del 2018
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="259">
   <si>
     <t>Expediente</t>
   </si>
@@ -801,6 +801,12 @@
   </si>
   <si>
     <t>416 GB</t>
+  </si>
+  <si>
+    <t>598 GB</t>
+  </si>
+  <si>
+    <t>332 GB</t>
   </si>
 </sst>
 </file>
@@ -2403,10 +2409,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2572,6 +2578,26 @@
       </c>
       <c r="F7" s="1">
         <v>43391</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8">
+        <v>1123</v>
+      </c>
+      <c r="C8">
+        <v>499</v>
+      </c>
+      <c r="D8" t="s">
+        <v>257</v>
+      </c>
+      <c r="E8" t="s">
+        <v>258</v>
+      </c>
+      <c r="F8" s="1">
+        <v>43430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Respaldo al 12/12/2018 y cambio de cabecera
respaldo al 12/12/2018 y cambie la columna dias por expedientes.
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="263">
   <si>
     <t>Expediente</t>
   </si>
@@ -362,9 +362,6 @@
     <t>Cantidad de Archivos</t>
   </si>
   <si>
-    <t>Dias</t>
-  </si>
-  <si>
     <t>Espacio Ocupado</t>
   </si>
   <si>
@@ -813,6 +810,15 @@
   </si>
   <si>
     <t>249 GB</t>
+  </si>
+  <si>
+    <t>Expedientes</t>
+  </si>
+  <si>
+    <t>684 GB</t>
+  </si>
+  <si>
+    <t>246 GB</t>
   </si>
 </sst>
 </file>
@@ -1903,7 +1909,7 @@
         <v>96</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2274,7 +2280,7 @@
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19" s="10">
         <v>43293</v>
@@ -2291,7 +2297,7 @@
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20" s="10">
         <v>43293</v>
@@ -2308,7 +2314,7 @@
     </row>
     <row r="21" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21" s="10">
         <v>43293</v>
@@ -2320,12 +2326,12 @@
         <v>0.46111111111111108</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22" s="10">
         <v>43293</v>
@@ -2342,7 +2348,7 @@
     </row>
     <row r="23" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B23" s="10">
         <v>43293</v>
@@ -2359,7 +2365,7 @@
     </row>
     <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B24" s="10">
         <v>43293</v>
@@ -2371,7 +2377,7 @@
         <v>0.48888888888888887</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -2388,12 +2394,12 @@
         <v>0.44444444444444442</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B26" s="10">
         <v>43298</v>
@@ -2405,7 +2411,7 @@
         <v>0.43888888888888888</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2415,10 +2421,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2438,24 +2444,24 @@
         <v>109</v>
       </c>
       <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
         <v>110</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>111</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>112</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>113</v>
-      </c>
-      <c r="G1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2">
         <v>826</v>
@@ -2464,10 +2470,10 @@
         <v>196</v>
       </c>
       <c r="D2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" t="s">
         <v>116</v>
-      </c>
-      <c r="E2" t="s">
-        <v>117</v>
       </c>
       <c r="F2" s="1">
         <v>43292</v>
@@ -2478,7 +2484,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3">
         <v>822</v>
@@ -2487,21 +2493,21 @@
         <v>196</v>
       </c>
       <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
         <v>119</v>
-      </c>
-      <c r="E3" t="s">
-        <v>120</v>
       </c>
       <c r="F3" s="1">
         <v>43292</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4">
         <v>878</v>
@@ -2510,10 +2516,10 @@
         <v>256</v>
       </c>
       <c r="D4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" t="s">
         <v>251</v>
-      </c>
-      <c r="E4" t="s">
-        <v>252</v>
       </c>
       <c r="F4" s="1">
         <v>43335</v>
@@ -2524,7 +2530,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5">
         <v>851</v>
@@ -2533,21 +2539,21 @@
         <v>230</v>
       </c>
       <c r="D5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" t="s">
         <v>137</v>
-      </c>
-      <c r="E5" t="s">
-        <v>138</v>
       </c>
       <c r="F5" s="1">
         <v>43322</v>
       </c>
       <c r="G5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6">
         <v>952</v>
@@ -2556,10 +2562,10 @@
         <v>317</v>
       </c>
       <c r="D6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" t="s">
         <v>253</v>
-      </c>
-      <c r="E6" t="s">
-        <v>254</v>
       </c>
       <c r="F6" s="1">
         <v>43371</v>
@@ -2568,7 +2574,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7">
         <v>1015</v>
@@ -2577,10 +2583,10 @@
         <v>387</v>
       </c>
       <c r="D7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7" t="s">
         <v>255</v>
-      </c>
-      <c r="E7" t="s">
-        <v>256</v>
       </c>
       <c r="F7" s="1">
         <v>43391</v>
@@ -2588,7 +2594,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8">
         <v>1123</v>
@@ -2597,10 +2603,10 @@
         <v>499</v>
       </c>
       <c r="D8" t="s">
+        <v>256</v>
+      </c>
+      <c r="E8" t="s">
         <v>257</v>
-      </c>
-      <c r="E8" t="s">
-        <v>258</v>
       </c>
       <c r="F8" s="1">
         <v>43430</v>
@@ -2608,7 +2614,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9">
         <v>1166</v>
@@ -2617,13 +2623,33 @@
         <v>547</v>
       </c>
       <c r="D9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E9" t="s">
         <v>259</v>
-      </c>
-      <c r="E9" t="s">
-        <v>260</v>
       </c>
       <c r="F9" s="1">
         <v>43444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10">
+        <v>1171</v>
+      </c>
+      <c r="C10">
+        <v>554</v>
+      </c>
+      <c r="D10" t="s">
+        <v>261</v>
+      </c>
+      <c r="E10" t="s">
+        <v>262</v>
+      </c>
+      <c r="F10" s="1">
+        <v>43446</v>
       </c>
     </row>
   </sheetData>
@@ -3117,7 +3143,7 @@
         <v>71</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -3180,7 +3206,7 @@
         <v>43298</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C21" s="4">
         <v>43216</v>
@@ -3195,7 +3221,7 @@
         <v>13</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>100</v>
@@ -3360,16 +3386,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -3644,7 +3670,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B20" s="13">
         <v>43256</v>
@@ -3659,7 +3685,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" s="13">
         <v>43256</v>
@@ -3689,7 +3715,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" s="13">
         <v>43223</v>
@@ -3704,7 +3730,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B24" s="13">
         <v>43223</v>
@@ -3719,7 +3745,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B25" s="13">
         <v>43223</v>
@@ -3734,7 +3760,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B26" s="13">
         <v>43223</v>
@@ -3749,7 +3775,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B27" s="13">
         <v>43228</v>
@@ -3764,7 +3790,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B28" s="13">
         <v>43228</v>
@@ -3779,7 +3805,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B29" s="13">
         <v>43228</v>
@@ -3794,7 +3820,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B30" s="13">
         <v>43228</v>
@@ -3809,7 +3835,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B31" s="13">
         <v>43228</v>
@@ -3819,12 +3845,12 @@
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B32" s="13">
         <v>43228</v>
@@ -3854,7 +3880,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B34" s="13">
         <v>43229</v>
@@ -3869,7 +3895,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B35" s="13">
         <v>43229</v>
@@ -3884,7 +3910,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B36" s="13">
         <v>43229</v>
@@ -3899,7 +3925,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B37" s="13">
         <v>43229</v>
@@ -3959,7 +3985,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B41" s="13">
         <v>43235</v>
@@ -3974,7 +4000,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B42" s="13">
         <v>43235</v>
@@ -3989,7 +4015,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B43" s="13">
         <v>43235</v>
@@ -4004,7 +4030,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B44" s="13">
         <v>43237</v>
@@ -4019,7 +4045,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B45" s="13">
         <v>43237</v>
@@ -4034,7 +4060,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B46" s="13">
         <v>43237</v>
@@ -4049,7 +4075,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B47" s="13">
         <v>43237</v>
@@ -4064,7 +4090,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B48" s="13">
         <v>43237</v>
@@ -4074,12 +4100,12 @@
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B49" s="13">
         <v>43242</v>
@@ -4094,7 +4120,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B50" s="13">
         <v>43242</v>
@@ -4119,12 +4145,12 @@
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B52" s="13">
         <v>43242</v>
@@ -4149,7 +4175,7 @@
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
@@ -4169,7 +4195,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B55" s="13">
         <v>43244</v>
@@ -4184,7 +4210,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B56" s="13">
         <v>43244</v>
@@ -4199,7 +4225,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B57" s="13">
         <v>43244</v>
@@ -4214,7 +4240,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B58" s="13">
         <v>43244</v>
@@ -4229,7 +4255,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B59" s="13">
         <v>43244</v>
@@ -4244,7 +4270,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B60" s="13">
         <v>43244</v>
@@ -4259,7 +4285,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B61" s="13">
         <v>43249</v>
@@ -4274,7 +4300,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B62" s="13">
         <v>43249</v>
@@ -4289,7 +4315,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B63" s="13">
         <v>43249</v>
@@ -4304,7 +4330,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B64" s="13">
         <v>43249</v>
@@ -4319,7 +4345,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B65" s="13">
         <v>43249</v>
@@ -4334,7 +4360,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B66" s="13">
         <v>43251</v>
@@ -4349,7 +4375,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B67" s="13">
         <v>43251</v>
@@ -4364,7 +4390,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B68" s="13">
         <v>43251</v>
@@ -4379,7 +4405,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B69" s="13">
         <v>43251</v>
@@ -4394,7 +4420,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B70" s="13">
         <v>43251</v>
@@ -4409,7 +4435,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B71" s="13">
         <v>43251</v>
@@ -4424,7 +4450,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B72" s="13">
         <v>43251</v>
@@ -4439,7 +4465,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B73" s="13">
         <v>43192</v>
@@ -4454,7 +4480,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B74" s="13">
         <v>43193</v>
@@ -4469,7 +4495,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B75" s="13">
         <v>43193</v>
@@ -4477,12 +4503,12 @@
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
       <c r="E75" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B76" s="13">
         <v>43193</v>
@@ -4497,7 +4523,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B77" s="13">
         <v>43193</v>
@@ -4512,7 +4538,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B78" s="13">
         <v>43193</v>
@@ -4527,7 +4553,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B79" s="13">
         <v>43195</v>
@@ -4542,7 +4568,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B80" s="13">
         <v>43195</v>
@@ -4557,7 +4583,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B81" s="13">
         <v>43195</v>
@@ -4572,7 +4598,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B82" s="13">
         <v>43195</v>
@@ -4587,7 +4613,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B83" s="13">
         <v>43200</v>
@@ -4602,7 +4628,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B84" s="13">
         <v>43200</v>
@@ -4617,7 +4643,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B85" s="13">
         <v>43200</v>
@@ -4632,7 +4658,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B86" s="13">
         <v>43202</v>
@@ -4647,7 +4673,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B87" s="13">
         <v>43202</v>
@@ -4662,7 +4688,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B88" s="13">
         <v>43202</v>
@@ -4677,7 +4703,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B89" s="13">
         <v>43202</v>
@@ -4707,7 +4733,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B91" s="13">
         <v>43202</v>
@@ -4722,7 +4748,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B92" s="13">
         <v>43207</v>
@@ -4737,7 +4763,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B93" s="13">
         <v>43207</v>
@@ -4752,7 +4778,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B94" s="13">
         <v>43207</v>
@@ -4767,7 +4793,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B95" s="13">
         <v>43207</v>
@@ -4782,7 +4808,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B96" s="13">
         <v>43209</v>
@@ -4790,12 +4816,12 @@
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
       <c r="E96" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B97" s="13">
         <v>43209</v>
@@ -4810,7 +4836,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B98" s="13">
         <v>43209</v>
@@ -4825,7 +4851,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B99" s="13">
         <v>43209</v>
@@ -4840,7 +4866,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B100" s="13">
         <v>43209</v>
@@ -4855,7 +4881,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B101" s="13">
         <v>43209</v>
@@ -4870,7 +4896,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B102" s="13">
         <v>43214</v>
@@ -4885,7 +4911,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B103" s="13">
         <v>43214</v>
@@ -4900,7 +4926,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B104" s="13">
         <v>43214</v>
@@ -4915,7 +4941,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B105" s="13">
         <v>43214</v>
@@ -4930,7 +4956,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B106" s="13">
         <v>43216</v>
@@ -4938,12 +4964,12 @@
       <c r="C106" s="12"/>
       <c r="D106" s="12"/>
       <c r="E106" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B107" s="13">
         <v>43216</v>
@@ -4958,7 +4984,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B108" s="13">
         <v>43216</v>
@@ -4966,12 +4992,12 @@
       <c r="C108" s="12"/>
       <c r="D108" s="12"/>
       <c r="E108" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B109" s="13">
         <v>43216</v>
@@ -4986,7 +5012,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B110" s="13">
         <v>43216</v>
@@ -5001,7 +5027,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B111" s="13">
         <v>43216</v>
@@ -5016,7 +5042,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B112" s="13">
         <v>43216</v>
@@ -5031,7 +5057,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B113" s="13">
         <v>43160</v>
@@ -5046,7 +5072,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B114" s="13">
         <v>43160</v>
@@ -5061,7 +5087,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B115" s="13">
         <v>43160</v>
@@ -5076,7 +5102,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B116" s="13">
         <v>43160</v>
@@ -5091,7 +5117,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B117" s="13">
         <v>43165</v>
@@ -5106,7 +5132,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B118" s="13">
         <v>43165</v>
@@ -5121,7 +5147,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B119" s="13">
         <v>43165</v>
@@ -5136,7 +5162,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B120" s="13">
         <v>43165</v>
@@ -5144,12 +5170,12 @@
       <c r="C120" s="12"/>
       <c r="D120" s="12"/>
       <c r="E120" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B121" s="13">
         <v>43165</v>
@@ -5164,7 +5190,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B122" s="13">
         <v>43165</v>
@@ -5179,7 +5205,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B123" s="13">
         <v>43167</v>
@@ -5194,7 +5220,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B124" s="13">
         <v>43167</v>
@@ -5209,7 +5235,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B125" s="13">
         <v>43167</v>
@@ -5224,7 +5250,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B126" s="13">
         <v>43167</v>
@@ -5239,7 +5265,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B127" s="13">
         <v>43167</v>
@@ -5254,7 +5280,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B128" s="13">
         <v>43172</v>
@@ -5262,12 +5288,12 @@
       <c r="C128" s="12"/>
       <c r="D128" s="12"/>
       <c r="E128" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B129" s="13">
         <v>43172</v>
@@ -5282,7 +5308,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B130" s="13">
         <v>43172</v>
@@ -5297,7 +5323,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B131" s="13">
         <v>43172</v>
@@ -5305,12 +5331,12 @@
       <c r="C131" s="12"/>
       <c r="D131" s="12"/>
       <c r="E131" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B132" s="13">
         <v>43172</v>
@@ -5325,7 +5351,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B133" s="13">
         <v>43172</v>
@@ -5340,7 +5366,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B134" s="13">
         <v>43174</v>
@@ -5355,7 +5381,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B135" s="13">
         <v>43174</v>
@@ -5370,7 +5396,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B136" s="13">
         <v>43174</v>
@@ -5385,7 +5411,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B137" s="13">
         <v>43174</v>
@@ -5400,7 +5426,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B138" s="13">
         <v>43174</v>
@@ -5415,7 +5441,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B139" s="13">
         <v>43174</v>
@@ -5423,12 +5449,12 @@
       <c r="C139" s="12"/>
       <c r="D139" s="12"/>
       <c r="E139" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B140" s="13">
         <v>43179</v>
@@ -5443,7 +5469,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B141" s="13">
         <v>43179</v>
@@ -5458,7 +5484,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B142" s="13">
         <v>43179</v>
@@ -5473,7 +5499,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B143" s="13">
         <v>43179</v>
@@ -5488,7 +5514,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B144" s="13">
         <v>43179</v>
@@ -5503,7 +5529,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B145" s="13">
         <v>43179</v>
@@ -5518,7 +5544,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B146" s="13">
         <v>43181</v>
@@ -5533,7 +5559,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B147" s="13">
         <v>43181</v>
@@ -5548,7 +5574,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B148" s="13">
         <v>43181</v>
@@ -5563,7 +5589,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B149" s="13">
         <v>43181</v>
@@ -5578,7 +5604,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B150" s="13">
         <v>43181</v>
@@ -5616,21 +5642,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2" s="13">
         <v>43228</v>
@@ -5638,12 +5664,12 @@
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" s="13">
         <v>43237</v>
@@ -5651,7 +5677,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -5664,7 +5690,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -5677,12 +5703,12 @@
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6" s="13">
         <v>43193</v>
@@ -5690,12 +5716,12 @@
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B7" s="13">
         <v>43209</v>
@@ -5703,12 +5729,12 @@
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B8" s="13">
         <v>43216</v>
@@ -5716,12 +5742,12 @@
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9" s="13">
         <v>43216</v>
@@ -5729,12 +5755,12 @@
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B10" s="13">
         <v>43165</v>
@@ -5742,12 +5768,12 @@
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B11" s="13">
         <v>43172</v>
@@ -5755,12 +5781,12 @@
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B12" s="13">
         <v>43172</v>
@@ -5768,12 +5794,12 @@
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B13" s="13">
         <v>43174</v>
@@ -5781,7 +5807,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Respaldo al dia 19/12/2018
respaldo las audiencias al dia 19/12/2018.
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="267">
   <si>
     <t>Expediente</t>
   </si>
@@ -821,13 +821,16 @@
     <t>246 GB</t>
   </si>
   <si>
-    <t>14/14/2018</t>
-  </si>
-  <si>
     <t>688 GB</t>
   </si>
   <si>
     <t>242 GB</t>
+  </si>
+  <si>
+    <t>703 GB</t>
+  </si>
+  <si>
+    <t>227 GB</t>
   </si>
 </sst>
 </file>
@@ -912,7 +915,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -2433,10 +2436,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2675,13 +2678,33 @@
         <v>564</v>
       </c>
       <c r="D11" t="s">
+        <v>263</v>
+      </c>
+      <c r="E11" t="s">
         <v>264</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="15">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12">
+        <v>1191</v>
+      </c>
+      <c r="C12">
+        <v>576</v>
+      </c>
+      <c r="D12" t="s">
         <v>265</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>263</v>
+      <c r="E12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F12" s="1">
+        <v>43453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ACTUALIZACION DEL 25 DE ENERO DEL 2019
RESPALDO DE LAS AUDIENCIAS AL 25 DE ENERO DEL 2019
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="269">
   <si>
     <t>Expediente</t>
   </si>
@@ -831,6 +831,12 @@
   </si>
   <si>
     <t>227 GB</t>
+  </si>
+  <si>
+    <t>747 GB</t>
+  </si>
+  <si>
+    <t>183 GB</t>
   </si>
 </sst>
 </file>
@@ -2436,10 +2442,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2705,6 +2711,29 @@
       </c>
       <c r="F12" s="1">
         <v>43453</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13">
+        <v>1229</v>
+      </c>
+      <c r="C13">
+        <v>621</v>
+      </c>
+      <c r="D13" t="s">
+        <v>267</v>
+      </c>
+      <c r="E13" t="s">
+        <v>268</v>
+      </c>
+      <c r="F13" s="1">
+        <v>43490</v>
+      </c>
+      <c r="G13" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Respaldo dd al 13/03/2019
Respaldo del disco duro de las audiencias del mes de marzo del 2019
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="284">
   <si>
     <t>Expediente</t>
   </si>
@@ -876,6 +876,12 @@
   </si>
   <si>
     <t>151 GB</t>
+  </si>
+  <si>
+    <t>794 GB</t>
+  </si>
+  <si>
+    <t>137 GB</t>
   </si>
 </sst>
 </file>
@@ -2481,10 +2487,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2906,6 +2912,26 @@
       </c>
       <c r="F19" s="1">
         <v>43524</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20">
+        <v>1314</v>
+      </c>
+      <c r="C20">
+        <v>736</v>
+      </c>
+      <c r="D20" t="s">
+        <v>282</v>
+      </c>
+      <c r="E20" t="s">
+        <v>283</v>
+      </c>
+      <c r="F20" s="1">
+        <v>43537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Respaldo al disco duro al 01/04/2019
respaldo de marzo del 2019 y 01 de abril
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="286">
   <si>
     <t>Expediente</t>
   </si>
@@ -882,6 +882,12 @@
   </si>
   <si>
     <t>137 GB</t>
+  </si>
+  <si>
+    <t>817 GB</t>
+  </si>
+  <si>
+    <t>114 GB</t>
   </si>
 </sst>
 </file>
@@ -2487,10 +2493,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2932,6 +2938,26 @@
       </c>
       <c r="F20" s="1">
         <v>43537</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21">
+        <v>1356</v>
+      </c>
+      <c r="C21">
+        <v>787</v>
+      </c>
+      <c r="D21" t="s">
+        <v>284</v>
+      </c>
+      <c r="E21" t="s">
+        <v>285</v>
+      </c>
+      <c r="F21" s="1">
+        <v>43556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Respaldo al dia 10/04/2019
Respaldo al dia 04 de Abril del 2019
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="288">
   <si>
     <t>Expediente</t>
   </si>
@@ -888,6 +888,12 @@
   </si>
   <si>
     <t>114 GB</t>
+  </si>
+  <si>
+    <t>824 GB</t>
+  </si>
+  <si>
+    <t>106 GB</t>
   </si>
 </sst>
 </file>
@@ -2493,7 +2499,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
@@ -2958,6 +2964,26 @@
       </c>
       <c r="F21" s="1">
         <v>43556</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22">
+        <v>1371</v>
+      </c>
+      <c r="C22">
+        <v>807</v>
+      </c>
+      <c r="D22" t="s">
+        <v>286</v>
+      </c>
+      <c r="E22" t="s">
+        <v>287</v>
+      </c>
+      <c r="F22" s="1">
+        <v>43565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RESPALDO DE ABRIL DEL 2019
Respaldo al 30 de Abril
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="292">
   <si>
     <t>Expediente</t>
   </si>
@@ -900,6 +900,12 @@
   </si>
   <si>
     <t>103 GB</t>
+  </si>
+  <si>
+    <t>838 GB</t>
+  </si>
+  <si>
+    <t>92.8 GB</t>
   </si>
 </sst>
 </file>
@@ -2505,10 +2511,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3010,6 +3016,26 @@
       </c>
       <c r="F23" s="1">
         <v>43577</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24">
+        <v>1396</v>
+      </c>
+      <c r="C24">
+        <v>838</v>
+      </c>
+      <c r="D24" t="s">
+        <v>290</v>
+      </c>
+      <c r="E24" t="s">
+        <v>291</v>
+      </c>
+      <c r="F24" s="1">
+        <v>43585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Respaldo al dia 08/05/2019
Respaldo al 08/05/2019
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="294">
   <si>
     <t>Expediente</t>
   </si>
@@ -906,6 +906,12 @@
   </si>
   <si>
     <t>92.8 GB</t>
+  </si>
+  <si>
+    <t>848 GB</t>
+  </si>
+  <si>
+    <t>83 GB</t>
   </si>
 </sst>
 </file>
@@ -2511,10 +2517,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3036,6 +3042,26 @@
       </c>
       <c r="F24" s="1">
         <v>43585</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25">
+        <v>1410</v>
+      </c>
+      <c r="C25">
+        <v>856</v>
+      </c>
+      <c r="D25" t="s">
+        <v>292</v>
+      </c>
+      <c r="E25" t="s">
+        <v>293</v>
+      </c>
+      <c r="F25" s="1">
+        <v>43593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Respaldo Disco Duro 28/06/2019
Respaldo de Junio
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="302">
   <si>
     <t>Expediente</t>
   </si>
@@ -930,6 +930,12 @@
   </si>
   <si>
     <t>42.1 GB</t>
+  </si>
+  <si>
+    <t>931 GB</t>
+  </si>
+  <si>
+    <t>19.1 GB</t>
   </si>
 </sst>
 </file>
@@ -2535,10 +2541,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3140,6 +3146,26 @@
       </c>
       <c r="F28" s="1">
         <v>43626</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29">
+        <v>1509</v>
+      </c>
+      <c r="C29">
+        <v>978</v>
+      </c>
+      <c r="D29" t="s">
+        <v>300</v>
+      </c>
+      <c r="E29" t="s">
+        <v>301</v>
+      </c>
+      <c r="F29" s="1">
+        <v>43644</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Respaldo del mes de julio del 2019
respaldo al dia 19/07/2019
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="307">
   <si>
     <t>Expediente</t>
   </si>
@@ -942,6 +942,15 @@
   </si>
   <si>
     <t>9.93 GB</t>
+  </si>
+  <si>
+    <t>763 GB</t>
+  </si>
+  <si>
+    <t>168 GB</t>
+  </si>
+  <si>
+    <t>ELIMINE VIDEOS DE RESPALDO DE LA MEMORIA</t>
   </si>
 </sst>
 </file>
@@ -2547,10 +2556,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2914,7 +2923,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -2934,7 +2943,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>114</v>
       </c>
@@ -2954,7 +2963,7 @@
         <v>43503</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -2974,7 +2983,7 @@
         <v>43524</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>114</v>
       </c>
@@ -2994,7 +3003,7 @@
         <v>43537</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -3014,7 +3023,7 @@
         <v>43556</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>114</v>
       </c>
@@ -3034,7 +3043,7 @@
         <v>43565</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>114</v>
       </c>
@@ -3054,7 +3063,7 @@
         <v>43577</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>114</v>
       </c>
@@ -3074,7 +3083,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>114</v>
       </c>
@@ -3094,7 +3103,7 @@
         <v>43593</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>114</v>
       </c>
@@ -3114,7 +3123,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -3134,7 +3143,7 @@
         <v>43600</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -3154,7 +3163,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -3174,7 +3183,7 @@
         <v>43644</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>114</v>
       </c>
@@ -3192,6 +3201,29 @@
       </c>
       <c r="F30" s="1">
         <v>43656</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31">
+        <v>1540</v>
+      </c>
+      <c r="C31">
+        <v>1018</v>
+      </c>
+      <c r="D31" t="s">
+        <v>304</v>
+      </c>
+      <c r="E31" t="s">
+        <v>305</v>
+      </c>
+      <c r="F31" s="1">
+        <v>43665</v>
+      </c>
+      <c r="H31" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RESPALDO AL DIA 26/09/2019
Respaldo al dia 27 de Septiembre del 2019
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="313">
   <si>
     <t>Expediente</t>
   </si>
@@ -966,6 +966,9 @@
   </si>
   <si>
     <t>99.4 GB</t>
+  </si>
+  <si>
+    <t>82.2 GB</t>
   </si>
 </sst>
 </file>
@@ -2571,10 +2574,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3299,6 +3302,26 @@
       </c>
       <c r="F34" s="1">
         <v>43717</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35">
+        <v>1670</v>
+      </c>
+      <c r="C35">
+        <v>1186</v>
+      </c>
+      <c r="D35" t="s">
+        <v>294</v>
+      </c>
+      <c r="E35" t="s">
+        <v>312</v>
+      </c>
+      <c r="F35" s="1">
+        <v>43735</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RESPALDO HASTA OCTUBRE DEL 2019
RESPALDO HASTA EL 31/10/2019, SE LLENO EL DISCO DURO.
</commit_message>
<xml_diff>
--- a/relacion/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relacion/relación 4 oral pendientes de subir al sistema.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="316">
   <si>
     <t>Expediente</t>
   </si>
@@ -969,6 +969,15 @@
   </si>
   <si>
     <t>82.2 GB</t>
+  </si>
+  <si>
+    <t>28.8 GB</t>
+  </si>
+  <si>
+    <t>864 GB</t>
+  </si>
+  <si>
+    <t>SE LLENO EL DD RESPALDO HASTA OCTUBRE DEL 2019</t>
   </si>
 </sst>
 </file>
@@ -2574,10 +2583,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3264,7 +3273,7 @@
         <v>43684</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -3284,7 +3293,7 @@
         <v>43680</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>114</v>
       </c>
@@ -3304,7 +3313,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -3322,6 +3331,29 @@
       </c>
       <c r="F35" s="1">
         <v>43735</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36">
+        <v>1750</v>
+      </c>
+      <c r="C36">
+        <v>1277</v>
+      </c>
+      <c r="D36" t="s">
+        <v>314</v>
+      </c>
+      <c r="E36" t="s">
+        <v>313</v>
+      </c>
+      <c r="F36" s="1">
+        <v>43769</v>
+      </c>
+      <c r="H36" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>